<commit_message>
Identation, Reporter e Read.me
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="0" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="8160" yWindow="0" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>TestCase</t>
   </si>
@@ -92,12 +92,6 @@
     <t>TC1</t>
   </si>
   <si>
-    <t>TestName</t>
-  </si>
-  <si>
-    <t>LastTest</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>Carlos Gomes</t>
   </si>
   <si>
-    <t>122345@123456.com</t>
-  </si>
-  <si>
     <t>March</t>
   </si>
   <si>
@@ -141,6 +132,9 @@
   </si>
   <si>
     <t>18.51</t>
+  </si>
+  <si>
+    <t>testEmail@123456.com</t>
   </si>
 </sst>
 </file>
@@ -512,9 +506,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +557,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>9</v>
@@ -602,7 +596,7 @@
         <v>20</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -610,16 +604,16 @@
         <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F2" s="3">
         <v>123456</v>
@@ -628,40 +622,40 @@
         <v>8</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I2" s="3">
         <v>1991</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="Q2" s="3">
         <v>12345</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T2" s="3">
         <v>123456789</v>
@@ -670,10 +664,10 @@
         <v>987654321</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>